<commit_message>
refactor(q4): Rework question 4 to focus on active mobility and update political axis
</commit_message>
<xml_diff>
--- a/Docs/questionnaire-boussole-municipale-RC (rempli).xlsx
+++ b/Docs/questionnaire-boussole-municipale-RC (rempli).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EPelletier\Desktop\Boussole municipale\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A4065B-D6C3-4B23-B4A5-90D8CCE61713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2F631F-68A8-4D47-AFAC-3A89CEA1AD1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{DA823219-6DDE-4AA3-A422-E675866BABB5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DA823219-6DDE-4AA3-A422-E675866BABB5}"/>
   </bookViews>
   <sheets>
     <sheet name="questionnaire-parti-politique" sheetId="1" r:id="rId1"/>
@@ -1014,7 +1014,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1080,6 +1080,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1713,7 +1714,8 @@
       <c r="C24" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="2"/>
     </row>
     <row r="25" spans="2:6" ht="40.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>